<commit_message>
Dati modificati manualmente per avere la prima lettera di ogni indicatore maiuscola (serve per i titoli dei grafici).
Grafico leggermente migliorato: pallini più grandi, aggiunti titolo, legenda e nota sulla fonte. Ora i pallini sono colorati in base alla ripartizione geografica.
</commit_message>
<xml_diff>
--- a/captions.xlsx
+++ b/captions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\margh\LA MIA CARTELLA\DOTTORATO - Copia\Attività\Conferenze\StatisticAll 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/cstrozza_health_sdu_dk/Documents/_Other projects/StatisticAll 2021/IndicatoriDemografici/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E168B8-3CED-4120-A549-ADDA0E00A53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{D4E168B8-3CED-4120-A549-ADDA0E00A53D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{74671EA2-00F3-4562-B8BF-6B4E6AF69079}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E01B10D-EA2E-4DD7-911D-41406BCBAA7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E01B10D-EA2E-4DD7-911D-41406BCBAA7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,78 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
-    <t xml:space="preserve">tasso di natalità (per mille abitanti)                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tasso di mortalità (per mille abitanti)                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tasso di nuzialità (per mille abitanti)                                 </t>
-  </si>
-  <si>
-    <t>speranza di vita a 65 anni - totale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saldo migratorio interno (per mille abitanti)                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">saldo migratorio con l'estero (per mille abitanti)                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">saldo migratorio per altro motivo (per mille abitanti)                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">saldo migratorio totale (per mille abitanti)                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">crescita naturale (per mille abitanti)                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tasso di crescita totale (per mille abitanti)                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">numero medio di figli per donna                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">età media della madre al parto                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">speranza di vita alla nascita - maschi                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">speranza di vita a 65 anni - maschi                                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">speranza di vita alla nascita - femmine                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">speranza di vita a 65 anni - femmine                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">popolazione 0-14 anni al 1° gennaio (valori percentuali) - al 1° gennaio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">popolazione 15-64 anni (valori percentuali) - al 1° gennaio              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">popolazione 65 anni e più (valori percentuali) - al 1° gennaio           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">indice di dipendenza strutturale (valori percentuali) - al 1° gennaio    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">indice di dipendenza degli anziani (valori percentuali) - al 1° gennaio  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">indice di vecchiaia (valori percentuali) - al 1° gennaio                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">età media della popolazione - al 1° gennaio                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">speranza di vita alla nascita - totale                                   </t>
-  </si>
-  <si>
     <t>Il tasso di mortalità indica il numero di persone morte in un anno ogni 1.000 abitanti. Esso viene calcolato con riferimento alla popolazione media dell'anno determinata sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo e dividendo il risultato per due.</t>
   </si>
   <si>
@@ -127,6 +55,78 @@
   </si>
   <si>
     <t>indicatori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasso di natalità (per mille abitanti)                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasso di mortalità (per mille abitanti)                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasso di nuzialità (per mille abitanti)                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saldo migratorio interno (per mille abitanti)                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saldo migratorio con l'estero (per mille abitanti)                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saldo migratorio per altro motivo (per mille abitanti)                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saldo migratorio totale (per mille abitanti)                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crescita naturale (per mille abitanti)                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasso di crescita totale (per mille abitanti)                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numero medio di figli per donna                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età media della madre al parto                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speranza di vita alla nascita - maschi                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speranza di vita a 65 anni - maschi                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speranza di vita alla nascita - femmine                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speranza di vita a 65 anni - femmine                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popolazione 0-14 anni al 1° gennaio (valori percentuali) - al 1° gennaio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popolazione 15-64 anni (valori percentuali) - al 1° gennaio              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popolazione 65 anni e più (valori percentuali) - al 1° gennaio           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indice di dipendenza strutturale (valori percentuali) - al 1° gennaio    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indice di dipendenza degli anziani (valori percentuali) - al 1° gennaio  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indice di vecchiaia (valori percentuali) - al 1° gennaio                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età media della popolazione - al 1° gennaio                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speranza di vita alla nascita - totale                                   </t>
+  </si>
+  <si>
+    <t>Speranza di vita a 65 anni - totale</t>
   </si>
 </sst>
 </file>
@@ -175,7 +175,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -490,168 +490,168 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
     <col min="2" max="2" width="134" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B25" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modifiche captions + pagina introduttiva
</commit_message>
<xml_diff>
--- a/captions.xlsx
+++ b/captions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\margh\LA MIA CARTELLA\DOTTORATO - Copia\Attività\Conferenze\StatisticAll 2021\IndicatoriDemografici\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciglia88_ka/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BD396F-1067-47C4-8E59-C39C6955F5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994F2ADF-181C-954E-9221-F893EDA92146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E01B10D-EA2E-4DD7-911D-41406BCBAA7F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15480" xr2:uid="{8E01B10D-EA2E-4DD7-911D-41406BCBAA7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
-  <si>
-    <t>La crescita naturale è la differenza tra il tasso di natalità e il tasso di mortalità riferiti ad una determinata area e ad un certo lasso di tempo.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>descrizione indicatori</t>
   </si>
@@ -66,9 +63,6 @@
     <t xml:space="preserve">Saldo migratorio totale (per mille abitanti)                             </t>
   </si>
   <si>
-    <t xml:space="preserve">Crescita naturale (per mille abitanti)                                   </t>
-  </si>
-  <si>
     <t xml:space="preserve">Tasso di crescita totale (per mille abitanti)                            </t>
   </si>
   <si>
@@ -117,58 +111,75 @@
     <t>Speranza di vita a 65 anni - totale</t>
   </si>
   <si>
-    <t>Il tasso di natalità indica il numero di bambini nati vivi in un anno ogni 1000 abitanti. Viene calcolato con riferimento alla popolazione media dell'anno determinata sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo e dividendo il risultato per due.</t>
-  </si>
-  <si>
-    <t>Il tasso di mortalità indica il numero di persone morte in un anno ogni 1.000 abitanti. Viene calcolato con riferimento alla popolazione media dell'anno determinata sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo e dividendo il risultato per due.</t>
-  </si>
-  <si>
-    <t>Il tasso di nuzialità indica il numero dei matrimoni celebrati in un anno ogni 1000 abitanti. Viene calcolato con riferimento alla popolazione media dell'anno determinata sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo e dividendo il risultato per due.</t>
-  </si>
-  <si>
-    <t>Il saldo migratorio con l'estero è la differenza tra il numero degli iscritti nei registri anagrafici  per trasferimento di residenza dall'estero ed il numero dei cancellati per trasferimento di residenza all'estero.  Viene calcolato con riferimento alla popolazione media dell'anno, determinata sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo, dividendo il risultato per due e moliplicando per mille.</t>
-  </si>
-  <si>
-    <t>Il saldo migratorio totale è la differenza tra il numero degli iscritti ed il numero dei cancellati dai registri anagrafici per trasferimento di residenza. Viene calcolato con riferimento alla popolazione media dell'anno, determinata sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo, dividendo il risultato per due e moliplicando per mille.</t>
-  </si>
-  <si>
-    <t>Il tasso di crescita totale è il rapporto fra la variazione della popolazione in un dato anno (differenza fra popolazione al 31 dicembre e al 1° gennaio) e la popolazione media di quell'anno per mille individui. Si può calcolare come somma del tasso di crescita naturale e del tasso migratorio totale.</t>
-  </si>
-  <si>
-    <t>Età media al parto è l’età media al parto delle madri, espressa in anni e decimi di anno, calcolata considerando i soli nati vivi.</t>
-  </si>
-  <si>
-    <t>La speranza di vita alla nascita rappresenta il numero medio di anni che una persona può contare di vivere dalla nascita nell’ipotesi in cui, nel corso della propria esistenza, fosse sottoposta ai rischi di mortalità per età dell’anno di osservazione</t>
-  </si>
-  <si>
-    <t>La speranza di vita a 65 anni rappresenta  il numero medio di anni che una persona di 65 anni compiuti può contare di sopravvivere nell’ipotesi in cui, nel corso della successiva esistenza, fosse sottoposta ai rischi di mortalità per età (da 65 anni in su) dell’anno di osservazione.</t>
-  </si>
-  <si>
-    <t>Il numero medio di figli per donna (o tasso di fecondità totale - TFT) è il numero di figli che una donna metterebbe al mondo nel caso in cui, nel corso nella propria vita riproduttiva, fosse sottoposta al calendario di fecondità (sotto forma di tassi specifici di fecondità per età) dell’anno di osservazione.</t>
-  </si>
-  <si>
-    <t>La speranza di vita alla nascita rappresenta il numero medio di anni che una persona può contare di vivere dalla nascita nell’ipotesi in cui, nel corso della propria esistenza, fosse sottoposta ai rischi di mortalità per età dell’anno di osservazione.</t>
-  </si>
-  <si>
-    <t>Nell'analisi della struttura (o della distribuzione) per classi di età della popolazione, è la percentuale di popolazione in età 0-14 e fornisce un'indicazione del peso di tale gruppo relativamente all’insieme della popolazione.</t>
-  </si>
-  <si>
-    <t>Nell'analisi della struttura (o della distribuzione) per classi di età della popolazione, è la percentuale di popolazione in età 15-64 e fornisce un'indicazione del peso di tale gruppo relativamente all’insieme della popolazione.</t>
-  </si>
-  <si>
-    <t>Nell'analisi della struttura (o della distribuzione) per classi di età della popolazione, è la percentuale di popolazione con 65 anni o più e fornisce un'indicazione del peso di tale gruppo relativamente all’insieme della popolazione.</t>
-  </si>
-  <si>
-    <t>L'indice di dipendenza strutturale della popolazione è dato dal rapporto tra popolazione in età non attiva (0-14 anni e 65 anni e più) e popolazione in età attiva (15-64 anni), moltiplicato per 100</t>
-  </si>
-  <si>
-    <t>L'indice di dipendenza degli anziani è dato dal rapporto tra la popolazione di 65 anni e più e la popolazione in età attiva (15-64 anni), moltiplicato per 100.</t>
-  </si>
-  <si>
-    <t>L'indice di vecchiaia della popolazione è dato dal rapporto tra la popolazione di 65 anni e più e la popolazione di età 0-14 anni, moltiplicato per 100.</t>
-  </si>
-  <si>
-    <t>È l'età media della popolazione detenuta a una certa data, ottenuta dal rapporto tra la somma delle età di tutti gli individui e il numero degli individui, espressa in anni e decimi di anno.</t>
+    <t xml:space="preserve">Il tasso di natalità indica il numero di bambini nati vivi in un anno ogni 1000 abitanti. Viene calcolato dividendo il numero dei nati nell'anno per la popolazione media, ottenuta sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo, dividendo il risultato per due e moltiplicando per mille.
+Nel 2019 in Italia sono stati registrati 7 nuovi nati ogni 1000 abitanti. </t>
+  </si>
+  <si>
+    <t>Il tasso di nuzialità indica il numero dei matrimoni celebrati in un anno ogni 1000 abitanti. Viene calcolato dividendo il numero dei matrimoni nell'anno per la popolazione media, ottenuta sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo, dividendo il risultato per due e moltiplicando per mille.
+Nel 2019 in Italia si sono registrati 3,1 matrimoni ogni 1000 abitanti.</t>
+  </si>
+  <si>
+    <t>Il saldo migratorio con l'estero è la differenza tra il numero degli iscritti nei registri anagrafici  per trasferimento di residenza dall'estero ed il numero dei cancellati per trasferimento di residenza all'estero.  Viene calcolato con riferimento alla popolazione media dell'anno, determinata sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo, dividendo il risultato per due e moliplicando per mille.
+Nel 2019 in Italia si è registrato un saldo migratorio con l'estero positivo, con una media di 2,6 nuovi iscritti ogni 1000 abitanti residenti.</t>
+  </si>
+  <si>
+    <t>Crescita naturale (per mille abitanti)</t>
+  </si>
+  <si>
+    <t>Il numero medio di figli per donna (o tasso di fecondità totale - TFT) è dato dalla somma dei tassi specifici di fecondità calcolati rapportando, per ogni età feconda (15-49 anni), il numero dei nati vivi nell'anno di riferimento all’ammontare medio annuo della popolazione femminile. Nel 2019 in Italia si registra una media di 1,27 figli per donna, ben al di sotto della soglia di sostituzione pari a 2,1 figli per donna.</t>
+  </si>
+  <si>
+    <t>L'età media al parto è l’età media delle madri alla nascita dei figli, calcolata considerando i soli nati vivi. Nel 2019 l'età media della madre al primo figlio ha raggiunto i 32,1 anni.</t>
+  </si>
+  <si>
+    <t>Nell'analisi della struttura (o della distribuzione) per classi di età della popolazione, è la percentuale di popolazione in età 0-14 e fornisce un'indicazione del peso di tale gruppo relativamente all’insieme della popolazione. Nel 2019 in Italia gli individui di età compresa tra 0 e 14 anni rappresentavano il 13,2% della popolazione totale.</t>
+  </si>
+  <si>
+    <t>Nell'analisi della struttura (o della distribuzione) per classi di età della popolazione, è la percentuale di popolazione in età 15-64 e fornisce un'indicazione del peso di tale gruppo relativamente all’insieme della popolazione.  Nel 2019 in Italia gli individui di età compresa tra  14 e 65 anni rappresentavano il 64% della popolazione totale.</t>
+  </si>
+  <si>
+    <t>L'indice di vecchiaia della popolazione è dato dal rapporto tra la popolazione di 65 anni e più e la popolazione di età 0-14 anni, moltiplicato per 100. Nel 2019 in Italia si registrano 174 individui con 65 anni o più ogni 100 individui con età 0-14 anni.</t>
+  </si>
+  <si>
+    <t>Il tasso di mortalità indica il numero di persone morte in un anno ogni 1.000 abitanti. Viene calcolato dividendo il numero dei morti nell'anno per la popolazione media, ottenuta sommando la popolazione all'inizio del periodo con la popolazione alla fine del periodo, dividendo il risultato per due e moltiplicando per mille.
+Nel 2019 in Italia sono stati registrati poco meno di 10,6 morti ogni 1000 abitanti.</t>
+  </si>
+  <si>
+    <t>La crescita naturale della popolazione è la differenza tra il tasso di natalità e il tasso di mortalità, riferiti ad una determinata area e ad un certo lasso di tempo.
+Nel 2019 a livello nazionale continua il trend negativo della (de)crescita naturale, che si attesta a -3,6 per mille individui.</t>
+  </si>
+  <si>
+    <t>Il tasso di crescita totale è il rapporto fra la variazione della popolazione in un dato anno (differenza fra popolazione al 31 dicembre e al 1° gennaio) e la popolazione media di quell'anno per mille individui. Si può calcolare anche come somma del movimento naturale (nati meno morti) e del movimento migratorio (immigrati meno emigrati). Nel 2019 in Italia la popolazione è diminuita di 3,2 individui ogni 1000 abitanti.</t>
+  </si>
+  <si>
+    <t>La speranza di vita alla nascita rappresenta il numero medio di anni che una persona può contare di vivere dalla nascita nell’ipotesi in cui, nel corso della propria esistenza, fosse sottoposta ai rischi di mortalità per età dell’anno di osservazione. Un bambino nato nel 2019 in Italia può aspettarsi di vivere in media 81,1 anni.</t>
+  </si>
+  <si>
+    <t>La speranza di vita a 65 anni rappresenta  il numero medio di anni che una persona di 65 anni compiuti può contare di vivere nell’ipotesi in cui, nel corso della successiva esistenza, fosse sottoposta ai rischi di mortalità per età (da 65 anni in su) dell’anno di osservazione. Una donna che nel 2019 ha compiuto 65 anni, può aspettarsi di vivere in media altri 22,6 anni.</t>
+  </si>
+  <si>
+    <t>La speranza di vita alla nascita rappresenta il numero medio di anni che una persona può contare di vivere dalla nascita nell’ipotesi in cui, nel corso della propria esistenza, fosse sottoposta ai rischi di mortalità per età dell’anno di osservazione. Una bambina nata nel 2019, può aspettarsi di vivere in media 85,4 anni.</t>
+  </si>
+  <si>
+    <t>La speranza di vita a 65 anni rappresenta  il numero medio di anni che una persona di 65 anni compiuti può contare di vivere nell’ipotesi in cui, nel corso della successiva esistenza, fosse sottoposta ai rischi di mortalità per età (da 65 anni in su) dell’anno di osservazione. Un uomo che nel 2019 ha compiuto 65 anni, può aspettarsi di vivere in media altri 19,4 anni.</t>
+  </si>
+  <si>
+    <t>La speranza di vita a 65 anni rappresenta  il numero medio di anni che una persona di 65 anni compiuti può contare di vivere nell’ipotesi in cui, nel corso della successiva esistenza, fosse sottoposta ai rischi di mortalità per età (da 65 anni in su) dell’anno di osservazione.  Un individuo (maschio o femmina) che nel 2019 ha compiuto 65 anni, può aspettarsi di vivere in media altri 21 anni.</t>
+  </si>
+  <si>
+    <t>La speranza di vita alla nascita rappresenta il numero medio di anni che una persona può contare di vivere dalla nascita nell’ipotesi in cui, nel corso della propria esistenza, fosse sottoposta ai rischi di mortalità per età dell’anno di osservazione.  Un bambino (maschio o femmina) nato nel 2019 in Italia può aspettarsi di vivere in media 83,2 anni.</t>
+  </si>
+  <si>
+    <t>Nell'analisi della struttura (o della distribuzione) per classi di età della popolazione, è la percentuale di popolazione con 65 anni o più e fornisce un'indicazione del peso di tale gruppo relativamente all’insieme della popolazione. Nel 2019 in Italia gli individui con 65 anni o più rappresentavano il 22,9% della popolazione totale.</t>
+  </si>
+  <si>
+    <t>L'indice di dipendenza strutturale della popolazione è dato dal rapporto tra popolazione in età non attiva (0-14 anni e 65 anni e più) e popolazione in età attiva (15-64 anni), moltiplicato per 100. Nel 2019 a livello nazionale si registrano 56,4 individui in età non attiva (tra bambini under-14 e anziani over-65) ogni 100 persone in età attiva.</t>
+  </si>
+  <si>
+    <t>L'indice di dipendenza degli anziani è dato dal rapporto tra la popolazione di 65 anni e più e la popolazione in età attiva (15-64 anni), moltiplicato per 100. Nel 2019 a livello nazionale si registrano 35,8 individui di 65 anni o più ogni 100 persone in età attiva.</t>
+  </si>
+  <si>
+    <t>L'età media della popolazione a una certa data è ottenuta dal rapporto tra la somma delle età di tutti gli individui e il numero totale degli individui. Nel 2019 in Italia l'età media della popolazione ha raggiunto i 45,5 anni.</t>
   </si>
 </sst>
 </file>
@@ -212,9 +223,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -531,208 +549,205 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC893BF-D5C5-4FA9-8452-D6FA45433575}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
-    <col min="2" max="2" width="134" customWidth="1"/>
+    <col min="2" max="2" width="134" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="12" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="18" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="19" spans="1:2" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="23" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>